<commit_message>
Mise a jour des documents
</commit_message>
<xml_diff>
--- a/Documents/Phase de Lancement/Planning_Des_Phases.xlsx
+++ b/Documents/Phase de Lancement/Planning_Des_Phases.xlsx
@@ -824,7 +824,7 @@
   <dimension ref="B2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,7 +896,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F5" s="6">
         <v>3</v>

</xml_diff>